<commit_message>
Manque comparatif de base et apres je commence les modif
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29E6AC6-D99C-4095-BB89-69C790464563}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB179BF-202E-4103-A5A6-7823AD1D6349}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
   <si>
     <t>Catégorie</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ligne 48 / 49  Element &lt;li&gt; vide, ne sert à rien </t>
+  </si>
+  <si>
+    <t>SEO (Indexation)</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -483,13 +486,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -499,6 +502,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -819,11 +825,12 @@
   <dimension ref="B1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="4" width="37.85546875" customWidth="1"/>
@@ -1207,7 +1214,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="17" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1227,7 +1234,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="9"/>
+      <c r="F32" s="17"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1316,7 +1323,9 @@
       <c r="E40" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="G40" s="5" t="s">
         <v>84</v>
       </c>
@@ -1360,67 +1369,67 @@
     </row>
     <row r="46" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
       <c r="F49" s="14"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="14"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
       <c r="F51" s="14"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
       <c r="F52" s="14"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
       <c r="F53" s="14"/>
       <c r="G53" s="2"/>
     </row>
@@ -1470,67 +1479,67 @@
     </row>
     <row r="59" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="10"/>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
       <c r="F62" s="14"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
       <c r="F63" s="14"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
       <c r="F64" s="14"/>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
       <c r="F65" s="14"/>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
       <c r="F66" s="14"/>
       <c r="G66" s="2"/>
     </row>
@@ -1560,11 +1569,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C61:F61"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="C63:F63"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C50:F50"/>
     <mergeCell ref="C51:F51"/>
@@ -1573,12 +1583,11 @@
     <mergeCell ref="C59:F59"/>
     <mergeCell ref="C60:F60"/>
     <mergeCell ref="C58:F58"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C61:F61"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C63:F63"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C65:F65"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
2-Changement format BMP + redimension des img trop grandes
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC054DA-6816-4481-BA96-8EA335F5D76B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6345E400-CE6D-4E01-ACB6-33C86B73449F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -330,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,6 +358,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -495,7 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -504,9 +510,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -822,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
-  <dimension ref="B1:G69"/>
+  <dimension ref="B1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +846,7 @@
     <col min="7" max="7" width="66.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -859,7 +866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -878,8 +885,9 @@
       <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -887,7 +895,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:7" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -906,8 +914,9 @@
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -915,7 +924,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:7" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -935,7 +944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -943,7 +952,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -961,7 +970,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -969,7 +978,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="2:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -989,7 +998,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -997,8 +1006,8 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1006,7 +1015,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
@@ -1024,7 +1033,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1214,7 +1223,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="17" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1234,7 +1243,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="14"/>
+      <c r="F32" s="17"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1369,28 +1378,28 @@
     </row>
     <row r="46" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1479,28 +1488,28 @@
     </row>
     <row r="59" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="10"/>
-      <c r="C59" s="17" t="s">
+      <c r="C59" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1569,6 +1578,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C50:F50"/>
     <mergeCell ref="C51:F51"/>
@@ -1582,12 +1597,6 @@
     <mergeCell ref="C63:F63"/>
     <mergeCell ref="C64:F64"/>
     <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
3-Remplacement d'images par des textes
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6345E400-CE6D-4E01-ACB6-33C86B73449F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175BB9AA-498E-4A52-9B59-5A43B6F1FF21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -492,6 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -501,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -510,10 +511,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -832,7 +832,7 @@
   <dimension ref="B1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +885,7 @@
       <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="18"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
@@ -914,7 +914,7 @@
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="18"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -943,6 +943,7 @@
       <c r="G7" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="H7" s="11"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
@@ -1223,7 +1224,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="15" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1243,7 +1244,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="17"/>
+      <c r="F32" s="15"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1368,78 +1369,78 @@
       <c r="B45" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
       <c r="G45" s="2"/>
     </row>
     <row r="46" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="13"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="14"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="13"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="14"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="13"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="14"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="13"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="14"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="13"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="14"/>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
@@ -1478,78 +1479,78 @@
       <c r="B58" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
       <c r="G58" s="2"/>
     </row>
     <row r="59" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="10"/>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="13"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="14"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="13"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="14"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="13"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="14"/>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="13"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="14"/>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="13"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="14"/>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
@@ -1578,12 +1579,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C50:F50"/>
     <mergeCell ref="C51:F51"/>
@@ -1597,6 +1592,12 @@
     <mergeCell ref="C63:F63"/>
     <mergeCell ref="C64:F64"/>
     <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
4-Ajout de balises strong
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175BB9AA-498E-4A52-9B59-5A43B6F1FF21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F8B3AE-C2F9-44F2-ABB5-AA2D3409215F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -502,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,7 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -832,7 +832,7 @@
   <dimension ref="B1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,6 +970,7 @@
       <c r="G9" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -1224,7 +1225,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1244,7 +1245,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="15"/>
+      <c r="F32" s="18"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1379,28 +1380,28 @@
     </row>
     <row r="46" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1489,28 +1490,28 @@
     </row>
     <row r="59" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="10"/>
-      <c r="C59" s="18" t="s">
+      <c r="C59" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1579,6 +1580,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C50:F50"/>
     <mergeCell ref="C51:F51"/>
@@ -1592,12 +1599,6 @@
     <mergeCell ref="C63:F63"/>
     <mergeCell ref="C64:F64"/>
     <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
5-Supression des liens annuaires + mise en place des liens partenaires
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F8B3AE-C2F9-44F2-ABB5-AA2D3409215F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3726D6E8-6344-4A1B-AD96-1976337AE51F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -502,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,7 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -832,7 +832,7 @@
   <dimension ref="B1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,6 +999,7 @@
       <c r="G11" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
@@ -1225,7 +1226,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="15" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1245,7 +1246,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="18"/>
+      <c r="F32" s="15"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1380,28 +1381,28 @@
     </row>
     <row r="46" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1490,28 +1491,28 @@
     </row>
     <row r="59" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="10"/>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1580,12 +1581,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C50:F50"/>
     <mergeCell ref="C51:F51"/>
@@ -1599,6 +1594,12 @@
     <mergeCell ref="C63:F63"/>
     <mergeCell ref="C64:F64"/>
     <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
6-Ajustement de la Keywords
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3726D6E8-6344-4A1B-AD96-1976337AE51F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406BA8E4-CAE0-4887-866E-BD7074B416A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -502,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,7 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
   <dimension ref="B1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,6 +1035,7 @@
       <c r="G15" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
@@ -1226,7 +1227,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1246,7 +1247,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="15"/>
+      <c r="F32" s="18"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1381,28 +1382,28 @@
     </row>
     <row r="46" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1491,28 +1492,28 @@
     </row>
     <row r="59" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="10"/>
-      <c r="C59" s="18" t="s">
+      <c r="C59" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1581,6 +1582,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C50:F50"/>
     <mergeCell ref="C51:F51"/>
@@ -1594,12 +1601,6 @@
     <mergeCell ref="C63:F63"/>
     <mergeCell ref="C64:F64"/>
     <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
8-Modif des H1 + H2
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C86CB7-0EFD-42DA-910B-514EB29D0F06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6327EF3-E8A5-49CC-9DC4-7AD1174D585A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
   <si>
     <t>Catégorie</t>
   </si>
@@ -301,6 +301,21 @@
   </si>
   <si>
     <t>SEO (Indexation)</t>
+  </si>
+  <si>
+    <t>h1 et p invisible</t>
+  </si>
+  <si>
+    <t>un h1 et un paragraphe ont étaients caché dans la page afin de tromper googlebot</t>
+  </si>
+  <si>
+    <t>Ne surtout pas tromper googlebot car il nous penalisera</t>
+  </si>
+  <si>
+    <t>http://www.seo-reference.net/optimisation/texte-cache.html</t>
+  </si>
+  <si>
+    <t>SEO (Black Hat)</t>
   </si>
 </sst>
 </file>
@@ -462,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -493,6 +508,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -502,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,9 +529,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -829,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
-  <dimension ref="B1:H69"/>
+  <dimension ref="B1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,6 +1112,7 @@
       <c r="G19" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -1228,7 +1248,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1248,7 +1268,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="15"/>
+      <c r="F32" s="19"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1283,37 +1303,39 @@
       <c r="E36" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="12" t="s">
         <v>75</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="2:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="2:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="G38" s="5" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -1321,27 +1343,25 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="F39" s="20"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="2:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>88</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="F40" s="20"/>
       <c r="G40" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
@@ -1352,7 +1372,26 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1361,106 +1400,99 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
+    <row r="44" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C47" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="10"/>
-      <c r="C46" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-      <c r="C47" s="18"/>
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="14"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="14"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="14"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="15"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="14"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="15"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="14"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="15"/>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="15"/>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="15"/>
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -1479,98 +1511,98 @@
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="7" t="s">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C60" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="10"/>
-      <c r="C59" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-      <c r="C60" s="18"/>
       <c r="D60" s="18"/>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="14"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="14"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="14"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="15"/>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="14"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="15"/>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="14"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="15"/>
       <c r="G66" s="2"/>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="15"/>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="15"/>
       <c r="G68" s="2"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
@@ -1581,27 +1613,43 @@
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
     </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C66:F66"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
     <mergeCell ref="C50:F50"/>
-    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C59:F59"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C58:F58"/>
+    <mergeCell ref="C54:F54"/>
+    <mergeCell ref="C55:F55"/>
     <mergeCell ref="C61:F61"/>
     <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C60:F60"/>
     <mergeCell ref="C63:F63"/>
     <mergeCell ref="C64:F64"/>
     <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C66:F66"/>
+    <mergeCell ref="C67:F67"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>
@@ -1619,8 +1667,8 @@
     <hyperlink ref="G31" r:id="rId13" xr:uid="{9BB06A1B-8CEE-43A1-BFE6-F29C506EF23C}"/>
     <hyperlink ref="G32" r:id="rId14" xr:uid="{C9FFC83B-907B-4E5E-A3A3-DDF921690623}"/>
     <hyperlink ref="G36" r:id="rId15" xr:uid="{A34EA9F6-F9AB-4839-A568-E5F5914C5181}"/>
-    <hyperlink ref="G38" r:id="rId16" xr:uid="{1951CD15-AE56-462F-B3C5-3D86082645C5}"/>
-    <hyperlink ref="G40" r:id="rId17" location=":~:text=Dans%20l'univers%20SEO%2C%20schema,Google%20et%20Yahoo%20entre%20autres).&amp;text=Cette%20op%C3%A9ration%20a%20pour%20but,dans%20leur%20approche%20d'indexation." display="https://www.journaldunet.fr/web-tech/dictionnaire-du-webmastering/1203519-schema-org-definition/#:~:text=Dans%20l'univers%20SEO%2C%20schema,Google%20et%20Yahoo%20entre%20autres).&amp;text=Cette%20op%C3%A9ration%20a%20pour%20but,dans%20leur%20approche%20d'indexation." xr:uid="{52C84F2B-0474-430C-8117-A86EE01746F9}"/>
+    <hyperlink ref="G40" r:id="rId16" xr:uid="{1951CD15-AE56-462F-B3C5-3D86082645C5}"/>
+    <hyperlink ref="G42" r:id="rId17" location=":~:text=Dans%20l'univers%20SEO%2C%20schema,Google%20et%20Yahoo%20entre%20autres).&amp;text=Cette%20op%C3%A9ration%20a%20pour%20but,dans%20leur%20approche%20d'indexation." display="https://www.journaldunet.fr/web-tech/dictionnaire-du-webmastering/1203519-schema-org-definition/#:~:text=Dans%20l'univers%20SEO%2C%20schema,Google%20et%20Yahoo%20entre%20autres).&amp;text=Cette%20op%C3%A9ration%20a%20pour%20but,dans%20leur%20approche%20d'indexation." xr:uid="{52C84F2B-0474-430C-8117-A86EE01746F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
10-Integration des balises Open Graph
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9870A4E7-4B36-4505-A647-D4CA1A39B08F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DF55FC-8F35-4048-A097-811CC19BD161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -521,7 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -530,7 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
   <dimension ref="B1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,6 +1166,7 @@
       <c r="G23" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
@@ -1249,7 +1250,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1269,7 +1270,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="17"/>
+      <c r="F32" s="20"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1432,28 +1433,28 @@
     </row>
     <row r="48" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1542,28 +1543,28 @@
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1632,6 +1633,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
     <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
@@ -1645,12 +1652,6 @@
     <mergeCell ref="C65:F65"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C67:F67"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
11-Favicon passé en png
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DF55FC-8F35-4048-A097-811CC19BD161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28060DB-B45B-4CFF-9299-07F9023FBCA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -521,7 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -530,7 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
   <dimension ref="B1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,6 +1193,7 @@
       <c r="G25" s="6" t="s">
         <v>56</v>
       </c>
+      <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
@@ -1250,7 +1251,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="17" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1270,7 +1271,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="20"/>
+      <c r="F32" s="17"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1433,28 +1434,28 @@
     </row>
     <row r="48" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1543,28 +1544,28 @@
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
-      <c r="C61" s="17" t="s">
+      <c r="C61" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1633,12 +1634,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
     <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
@@ -1652,6 +1647,12 @@
     <mergeCell ref="C65:F65"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C67:F67"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
12-Rendu visible le h1 h2 et p sur page Contact
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28060DB-B45B-4CFF-9299-07F9023FBCA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605A7745-E04F-4356-92A7-E3E7A65067DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -477,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -507,7 +507,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -521,16 +520,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -850,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
   <dimension ref="B1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +909,9 @@
       <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="11"/>
+      <c r="H3" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
@@ -913,6 +920,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -933,7 +941,9 @@
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="11"/>
+      <c r="H5" s="20">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -942,6 +952,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="2:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
@@ -962,7 +973,9 @@
       <c r="G7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="11"/>
+      <c r="H7" s="20">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
@@ -971,6 +984,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -989,7 +1003,9 @@
       <c r="G9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="H9" s="20">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -998,6 +1014,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -1018,7 +1035,9 @@
       <c r="G11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="20">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
@@ -1027,8 +1046,11 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="21"/>
+    </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1036,6 +1058,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="2:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
@@ -1054,7 +1077,9 @@
       <c r="G15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="11"/>
+      <c r="H15" s="20">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
@@ -1063,6 +1088,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
@@ -1083,7 +1109,9 @@
       <c r="G17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="20">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
@@ -1092,6 +1120,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
@@ -1112,7 +1141,9 @@
       <c r="G19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="11"/>
+      <c r="H19" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -1121,6 +1152,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
@@ -1139,7 +1171,9 @@
       <c r="G21" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="11"/>
+      <c r="H21" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
@@ -1148,6 +1182,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
@@ -1166,7 +1201,9 @@
       <c r="G23" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="11"/>
+      <c r="H23" s="20">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
@@ -1175,6 +1212,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
@@ -1193,7 +1231,9 @@
       <c r="G25" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H25" s="11"/>
+      <c r="H25" s="20">
+        <v>11</v>
+      </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
@@ -1202,6 +1242,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="2:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
@@ -1220,6 +1261,7 @@
       <c r="G27" s="5" t="s">
         <v>60</v>
       </c>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
@@ -1228,8 +1270,11 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="21"/>
+    </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1237,6 +1282,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
     </row>
     <row r="31" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
@@ -1251,12 +1297,13 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>66</v>
       </c>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
@@ -1271,29 +1318,34 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="17"/>
+      <c r="F32" s="19"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="21"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="2:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>71</v>
       </c>
@@ -1306,22 +1358,24 @@
       <c r="E36" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="11" t="s">
         <v>75</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="13"/>
+      <c r="F37" s="12"/>
       <c r="G37" s="5"/>
-    </row>
-    <row r="38" spans="2:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>71</v>
       </c>
@@ -1334,22 +1388,26 @@
       <c r="E38" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="11" t="s">
         <v>93</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="13"/>
+      <c r="F39" s="12"/>
       <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="2:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>71</v>
       </c>
@@ -1362,20 +1420,22 @@
       <c r="E40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F40" s="13"/>
+      <c r="F40" s="12"/>
       <c r="G40" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="2:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="2:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>71</v>
       </c>
@@ -1394,17 +1454,19 @@
       <c r="G42" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1412,7 +1474,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1420,82 +1482,82 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="C47" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="16"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="15"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="16"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="15"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="16"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="15"/>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="16"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="15"/>
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="16"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="15"/>
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -1534,78 +1596,78 @@
       <c r="B60" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="18" t="s">
+      <c r="C60" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15"/>
-      <c r="F64" s="16"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="15"/>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="16"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="15"/>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="16"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="15"/>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="16"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="15"/>
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="16"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="15"/>
       <c r="G68" s="2"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
@@ -1634,6 +1696,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
     <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
@@ -1647,12 +1715,6 @@
     <mergeCell ref="C65:F65"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C67:F67"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
13-Mise en place d'un schema.org
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605A7745-E04F-4356-92A7-E3E7A65067DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBBB481-C0F2-4397-BDC9-F28FBCF6EEFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
   <si>
     <t>Catégorie</t>
   </si>
@@ -294,12 +294,6 @@
     <t>Modification code:</t>
   </si>
   <si>
-    <t>Ligne 40 / 42  → Supprimé ces 2 Lignes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ligne 48 / 49  Element &lt;li&gt; vide, ne sert à rien </t>
-  </si>
-  <si>
     <t>SEO (Indexation)</t>
   </si>
   <si>
@@ -316,6 +310,15 @@
   </si>
   <si>
     <t>SEO (Black Hat)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ligne 58 / 59  Element &lt;li&gt; vide, ne sert à rien </t>
+  </si>
+  <si>
+    <t>Ligne 50 / 52  → Supprimé ces 2 Lignes</t>
+  </si>
+  <si>
+    <t>Renommer en page contact et mettre a jour les liens</t>
   </si>
 </sst>
 </file>
@@ -511,6 +514,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,12 +539,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -855,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
   <dimension ref="B1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +912,7 @@
       <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="13">
         <v>1</v>
       </c>
     </row>
@@ -941,7 +944,7 @@
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="13">
         <v>2</v>
       </c>
     </row>
@@ -973,7 +976,7 @@
       <c r="G7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="13">
         <v>3</v>
       </c>
     </row>
@@ -1003,7 +1006,7 @@
       <c r="G9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="13">
         <v>4</v>
       </c>
     </row>
@@ -1035,7 +1038,7 @@
       <c r="G11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1049,7 +1052,7 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H13" s="21"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
@@ -1077,7 +1080,7 @@
       <c r="G15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="13">
         <v>6</v>
       </c>
     </row>
@@ -1109,7 +1112,7 @@
       <c r="G17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="13">
         <v>7</v>
       </c>
     </row>
@@ -1141,7 +1144,7 @@
       <c r="G19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="13">
         <v>8</v>
       </c>
     </row>
@@ -1171,7 +1174,7 @@
       <c r="G21" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="13">
         <v>8</v>
       </c>
     </row>
@@ -1201,7 +1204,7 @@
       <c r="G23" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="20">
+      <c r="H23" s="13">
         <v>10</v>
       </c>
     </row>
@@ -1231,7 +1234,7 @@
       <c r="G25" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H25" s="20">
+      <c r="H25" s="13">
         <v>11</v>
       </c>
     </row>
@@ -1261,7 +1264,7 @@
       <c r="G27" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="20"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
@@ -1273,7 +1276,7 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H29" s="21"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
@@ -1297,7 +1300,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="21" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1318,7 +1321,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="19"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1334,7 +1337,7 @@
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H34" s="21"/>
+      <c r="H34" s="14"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
@@ -1380,21 +1383,21 @@
         <v>71</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="F38" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H38" s="20">
+      <c r="H38" s="13">
         <v>12</v>
       </c>
     </row>
@@ -1449,12 +1452,14 @@
         <v>83</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H42" s="2"/>
+      <c r="H42" s="13">
+        <v>13</v>
+      </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
@@ -1486,78 +1491,78 @@
       <c r="B47" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
+      <c r="C48" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="17"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="17"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="17"/>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="17"/>
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="17"/>
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -1596,78 +1601,80 @@
       <c r="B60" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
-      <c r="C61" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
+      <c r="C61" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
+      <c r="C62" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="17"/>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="15"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="17"/>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="15"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="17"/>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="17"/>
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="17"/>
       <c r="G68" s="2"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
14-Ajustement de la taille
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBBB481-C0F2-4397-BDC9-F28FBCF6EEFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6EC7F4-D6FE-438E-B719-5137B43A5E40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -529,7 +529,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -538,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
   <dimension ref="B1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,7 +1300,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="F31" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1321,7 +1321,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="18"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1367,7 +1367,9 @@
       <c r="G36" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="2"/>
+      <c r="H36" s="13">
+        <v>14</v>
+      </c>
     </row>
     <row r="37" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
@@ -1501,28 +1503,28 @@
     </row>
     <row r="48" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1611,30 +1613,30 @@
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
-      <c r="C61" s="18" t="s">
+      <c r="C61" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1703,12 +1705,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
     <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
@@ -1722,6 +1718,12 @@
     <mergeCell ref="C65:F65"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C67:F67"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
15-Mise en place d'un Formulaire correct et placement design bootstrap
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6EC7F4-D6FE-438E-B719-5137B43A5E40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F39D42-94D9-41B9-848D-92E606044897}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -258,9 +258,6 @@
     <t>La taille de la page n'est pas bien defini, elle depasse de l'ecran en responsiv</t>
   </si>
   <si>
-    <t>Ajuster comme il faut la taille de la page selon le périphérique utilisé</t>
-  </si>
-  <si>
     <t>Accessiblité</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>Renommer en page contact et mettre a jour les liens</t>
+  </si>
+  <si>
+    <t>Ajuster comme il faut la taille de la page selon le périphérique utilisé (Bootstrap mal appelé)</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,16 +529,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -858,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
   <dimension ref="B1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,7 +1303,7 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="21" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1321,7 +1324,7 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="18"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
@@ -1359,13 +1362,13 @@
         <v>73</v>
       </c>
       <c r="E36" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="G36" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="H36" s="13">
         <v>14</v>
@@ -1385,19 +1388,19 @@
         <v>71</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="H38" s="13">
         <v>12</v>
@@ -1417,19 +1420,21 @@
         <v>71</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H40" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="H40" s="13">
+        <v>15</v>
+      </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
@@ -1445,19 +1450,19 @@
         <v>71</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="F42" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="H42" s="13">
         <v>13</v>
@@ -1491,7 +1496,7 @@
     </row>
     <row r="47" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C47" s="19" t="s">
         <v>6</v>
@@ -1503,28 +1508,28 @@
     </row>
     <row r="48" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
+      <c r="C48" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1601,7 +1606,7 @@
     </row>
     <row r="60" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C60" s="19" t="s">
         <v>71</v>
@@ -1613,30 +1618,30 @@
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
-      <c r="C61" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D61" s="21"/>
-      <c r="E61" s="21"/>
-      <c r="F61" s="21"/>
+      <c r="C61" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
+      <c r="C62" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1705,6 +1710,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
     <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
@@ -1718,12 +1729,6 @@
     <mergeCell ref="C65:F65"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C67:F67"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
16-Minification de style.css / et-line.css / formhandler.js
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F39D42-94D9-41B9-848D-92E606044897}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED3E326-0CED-4299-86A8-6B7B5BF6DBDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="96">
   <si>
     <t>Catégorie</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>Ajuster comme il faut la taille de la page selon le périphérique utilisé (Bootstrap mal appelé)</t>
+  </si>
+  <si>
+    <t>minifier style,css/formHandler,js</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,20 +532,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -859,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
-  <dimension ref="B1:H71"/>
+  <dimension ref="B1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,6 +883,7 @@
     <col min="5" max="5" width="47.5703125" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" customWidth="1"/>
     <col min="7" max="7" width="66.85546875" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1096,7 +1106,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
@@ -1119,7 +1129,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1128,7 +1138,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>31</v>
       </c>
@@ -1151,7 +1161,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1160,7 +1170,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>44</v>
       </c>
@@ -1181,7 +1191,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1190,7 +1200,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>44</v>
       </c>
@@ -1211,7 +1221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1220,7 +1230,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>44</v>
       </c>
@@ -1241,7 +1251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1250,7 +1260,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="2:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>44</v>
       </c>
@@ -1269,7 +1279,7 @@
       </c>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1278,10 +1288,10 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1290,7 +1300,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>61</v>
       </c>
@@ -1303,15 +1313,20 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="F31" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="23">
+        <v>16</v>
+      </c>
+      <c r="I31" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>62</v>
       </c>
@@ -1324,11 +1339,11 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="18"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="2"/>
+      <c r="H32" s="23"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
@@ -1508,28 +1523,28 @@
     </row>
     <row r="48" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1628,20 +1643,20 @@
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,13 +1724,8 @@
       <c r="G71" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
+  <mergeCells count="20">
+    <mergeCell ref="H31:H32"/>
     <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
@@ -1729,6 +1739,12 @@
     <mergeCell ref="C65:F65"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C67:F67"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
16-Ne trouve pas comment concatener
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED3E326-0CED-4299-86A8-6B7B5BF6DBDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E68B682-3040-4179-B3BA-909CF9834E72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -321,7 +321,7 @@
     <t>Ajuster comme il faut la taille de la page selon le périphérique utilisé (Bootstrap mal appelé)</t>
   </si>
   <si>
-    <t>minifier style,css/formHandler,js</t>
+    <t>minifier style,css/formHandler,js et et-line,css</t>
   </si>
 </sst>
 </file>
@@ -523,6 +523,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -532,26 +538,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
   <dimension ref="B1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,16 +1313,16 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="23">
+      <c r="H31" s="16">
         <v>16</v>
       </c>
-      <c r="I31" s="24" t="s">
+      <c r="I31" s="15" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1339,11 +1339,11 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="18"/>
+      <c r="F32" s="24"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="23"/>
+      <c r="H32" s="16"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
@@ -1513,12 +1513,12 @@
       <c r="B47" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C47" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1549,42 +1549,42 @@
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="19"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="19"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="19"/>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="19"/>
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="19"/>
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -1623,22 +1623,22 @@
       <c r="B60" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
-      <c r="C61" s="22" t="s">
+      <c r="C61" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1661,42 +1661,42 @@
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="19"/>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="19"/>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="19"/>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="19"/>
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="19"/>
       <c r="G68" s="2"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
@@ -1725,6 +1725,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
     <mergeCell ref="H31:H32"/>
     <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
@@ -1741,10 +1745,6 @@
     <mergeCell ref="C67:F67"/>
     <mergeCell ref="C51:F51"/>
     <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
Ligne supprimé modif apporté
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E68B682-3040-4179-B3BA-909CF9834E72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52149697-BF67-4D2B-A82E-764BCCA611EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="100">
   <si>
     <t>Catégorie</t>
   </si>
@@ -312,9 +312,6 @@
     <t xml:space="preserve">Ligne 58 / 59  Element &lt;li&gt; vide, ne sert à rien </t>
   </si>
   <si>
-    <t>Ligne 50 / 52  → Supprimé ces 2 Lignes</t>
-  </si>
-  <si>
     <t>Renommer en page contact et mettre a jour les liens</t>
   </si>
   <si>
@@ -322,6 +319,21 @@
   </si>
   <si>
     <t>minifier style,css/formHandler,js et et-line,css</t>
+  </si>
+  <si>
+    <t>Ligne 63 → Supprimé le &amp;gt;</t>
+  </si>
+  <si>
+    <t>Ligne 115 → Supprimé le &amp;nbsp;</t>
+  </si>
+  <si>
+    <t>Ligne 50 / 52  → Supprimé ces 2 Lignes (keyword)</t>
+  </si>
+  <si>
+    <t>Ligne 256 → Supprimé la ligne keywords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ligne 60 / 61  Element &lt;li&gt; vide, ne sert à rien </t>
   </si>
 </sst>
 </file>
@@ -483,7 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -526,6 +538,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -541,16 +562,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -870,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
   <dimension ref="B1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,11 +1340,11 @@
       <c r="G31" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="16">
+      <c r="H31" s="19">
         <v>16</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1343,7 +1364,7 @@
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="16"/>
+      <c r="H32" s="19"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
@@ -1377,7 +1398,7 @@
         <v>73</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>74</v>
@@ -1513,78 +1534,86 @@
       <c r="B47" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
+      <c r="C48" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
+      <c r="C49" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
+      <c r="C50" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="19"/>
+      <c r="C51" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="27"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="19"/>
+      <c r="C52" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="19"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="22"/>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="19"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="22"/>
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="19"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="22"/>
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -1623,80 +1652,80 @@
       <c r="B60" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="22" t="s">
+      <c r="C60" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
+      <c r="C62" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="19"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="22"/>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="19"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="22"/>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="19"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="22"/>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="19"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="22"/>
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="19"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="22"/>
       <c r="G68" s="2"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
@@ -1725,11 +1754,8 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="F31:F32"/>
     <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
@@ -1743,8 +1769,11 @@
     <mergeCell ref="C65:F65"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C67:F67"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="H31:H32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
Modif sur desgin formulaire schema.org
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52149697-BF67-4D2B-A82E-764BCCA611EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5379B0E-514A-454D-939C-EB72BC7EED37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
   <si>
     <t>Catégorie</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ligne 60 / 61  Element &lt;li&gt; vide, ne sert à rien </t>
+  </si>
+  <si>
+    <t>Ligne 59 → Supprimé le &amp;gt;</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -538,40 +541,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -892,7 +892,7 @@
   <dimension ref="B1:I71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,13 +1334,13 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="19">
+      <c r="H31" s="26">
         <v>16</v>
       </c>
       <c r="I31" s="15" t="s">
@@ -1360,11 +1360,11 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="24"/>
+      <c r="F32" s="19"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="19"/>
+      <c r="H32" s="26"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
@@ -1534,12 +1534,12 @@
       <c r="B47" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1574,12 +1574,12 @@
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="27"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="18"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1652,12 +1652,12 @@
       <c r="B60" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1682,10 +1682,12 @@
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
+      <c r="C63" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1754,6 +1756,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="H31:H32"/>
     <mergeCell ref="C51:F51"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="C68:F68"/>
@@ -1770,10 +1776,6 @@
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C67:F67"/>
     <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="H31:H32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
Quelques modif et projet ok
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5379B0E-514A-454D-939C-EB72BC7EED37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FAB7E7-18B6-4C02-8260-2A1729BDACDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
   <si>
     <t>Catégorie</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>Ligne 59 → Supprimé le &amp;gt;</t>
+  </si>
+  <si>
+    <t>placer style css dans fichier css</t>
   </si>
 </sst>
 </file>
@@ -541,6 +544,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -562,16 +571,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -891,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
   <dimension ref="B1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,13 +1337,13 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="21" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="26">
+      <c r="H31" s="17">
         <v>16</v>
       </c>
       <c r="I31" s="15" t="s">
@@ -1360,11 +1363,11 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="19"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="26"/>
+      <c r="H32" s="17"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
@@ -1534,86 +1537,86 @@
       <c r="B47" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="23" t="s">
+      <c r="C48" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="23" t="s">
+      <c r="C49" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="23" t="s">
+      <c r="C50" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="18"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="20"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
-      <c r="C52" s="23" t="s">
+      <c r="C52" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="23"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="24"/>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="24"/>
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="24"/>
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -1652,82 +1655,84 @@
       <c r="B60" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="24" t="s">
+      <c r="C60" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="23"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="23" t="s">
+      <c r="C62" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="2"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="23" t="s">
+      <c r="C63" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="24"/>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="22"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="24"/>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="22"/>
+      <c r="C66" s="22"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="24"/>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="22"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="24"/>
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="24"/>
       <c r="G68" s="2"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
@@ -1756,12 +1761,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="F31:F32"/>
     <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
@@ -1775,6 +1774,12 @@
     <mergeCell ref="C65:F65"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C67:F67"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="F31:F32"/>
     <mergeCell ref="C47:F47"/>
   </mergeCells>
   <hyperlinks>

</xml_diff>

<commit_message>
Fini de modifier le code
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FAB7E7-18B6-4C02-8260-2A1729BDACDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A134FD-4910-4DD6-B4C6-2A2E37B9FC41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
   <si>
     <t>Catégorie</t>
   </si>
@@ -339,7 +339,16 @@
     <t>Ligne 59 → Supprimé le &amp;gt;</t>
   </si>
   <si>
-    <t>placer style css dans fichier css</t>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>Ligne 704 → Suppression du !important pour couleur h1 h2 h3 etc</t>
+  </si>
+  <si>
+    <t>Ligne 96 → Suppression de symbole incoherent</t>
+  </si>
+  <si>
+    <t>.tc-white → Suppression de important pour remplacer couleur</t>
   </si>
 </sst>
 </file>
@@ -369,7 +378,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +412,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,7 +516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -544,9 +559,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -562,20 +592,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -892,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
-  <dimension ref="B1:I71"/>
+  <dimension ref="B1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,13 +1358,13 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="F31" s="26" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="17">
+      <c r="H31" s="22">
         <v>16</v>
       </c>
       <c r="I31" s="15" t="s">
@@ -1363,11 +1384,11 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="26"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="17"/>
+      <c r="H32" s="22"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
@@ -1537,86 +1558,88 @@
       <c r="B47" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C47" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="18" t="s">
+      <c r="C51" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="20"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="25"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="24"/>
+      <c r="C53" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="25"/>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="24"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="18"/>
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="24"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="18"/>
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -1655,84 +1678,82 @@
       <c r="B60" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C60" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="26"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
-      <c r="C61" s="16" t="s">
+      <c r="C61" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="2" t="s">
-        <v>101</v>
-      </c>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="24"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="18"/>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="23"/>
-      <c r="F65" s="24"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="18"/>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
-      <c r="C66" s="22"/>
-      <c r="D66" s="23"/>
-      <c r="E66" s="23"/>
-      <c r="F66" s="24"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="18"/>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="24"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="18"/>
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="23"/>
-      <c r="E68" s="23"/>
-      <c r="F68" s="24"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="18"/>
       <c r="G68" s="2"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
@@ -1759,8 +1780,95 @@
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
     </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+    </row>
+    <row r="73" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="10"/>
+      <c r="C73" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+    </row>
+    <row r="74" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+      <c r="C74" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D74" s="27"/>
+      <c r="E74" s="27"/>
+      <c r="F74" s="27"/>
+    </row>
+    <row r="75" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="2"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="28"/>
+    </row>
+    <row r="76" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="2"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="18"/>
+    </row>
+    <row r="77" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="2"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="18"/>
+    </row>
+    <row r="78" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="2"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="18"/>
+    </row>
+    <row r="79" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="2"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="18"/>
+    </row>
+    <row r="80" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="29">
+    <mergeCell ref="C77:F77"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="C79:F79"/>
+    <mergeCell ref="C80:F80"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="C72:F72"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="C76:F76"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C47:F47"/>
     <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
@@ -1774,13 +1882,6 @@
     <mergeCell ref="C65:F65"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C67:F67"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C47:F47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>

</xml_diff>

<commit_message>
Fini avec Rapport Excel
</commit_message>
<xml_diff>
--- a/Audit-Analyse.xlsx
+++ b/Audit-Analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\chouetteagence\SimonBalleuxPruvost-4-09022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A134FD-4910-4DD6-B4C6-2A2E37B9FC41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6C25FE-D941-47B0-8FCD-A8F7FB37EFDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63EF069-1566-4467-92A2-BACFCEB750C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="115">
   <si>
     <t>Catégorie</t>
   </si>
@@ -349,13 +349,43 @@
   </si>
   <si>
     <t>.tc-white → Suppression de important pour remplacer couleur</t>
+  </si>
+  <si>
+    <t>Ajout d'une classe para pour h2 placement et hestétique</t>
+  </si>
+  <si>
+    <t>Ajout classe .citat pour taille des citations</t>
+  </si>
+  <si>
+    <t>Ajout classe .title p pour placemeent hestétique de paragraphe</t>
+  </si>
+  <si>
+    <t>Ajout de quelques strong</t>
+  </si>
+  <si>
+    <t>Ajout de classe .pos pour des placemenet</t>
+  </si>
+  <si>
+    <t>Ajou tde classe .foot pour alignement footer en flex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajou tde classe .pos2 pour placement </t>
+  </si>
+  <si>
+    <t>Ajou tde classe visible et visible2 pour titre caché page contact</t>
+  </si>
+  <si>
+    <t>Ajout de 2 classe size-center/size-descrip pour taille et couleur de different titres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout de classe color-h pour contrer un color imoprtant pour page accueil titre avant footer </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,8 +407,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,12 +450,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,7 +548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -559,24 +591,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -592,11 +609,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -913,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDFEC1-5B86-4B3C-856C-66E76D7338EB}">
-  <dimension ref="B1:I80"/>
+  <dimension ref="B1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,13 +1375,13 @@
       <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="21" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="22">
+      <c r="H31" s="17">
         <v>16</v>
       </c>
       <c r="I31" s="15" t="s">
@@ -1384,11 +1401,11 @@
       <c r="E32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="26"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="22"/>
+      <c r="H32" s="17"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
@@ -1558,88 +1575,88 @@
       <c r="B47" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="19" t="s">
+      <c r="C48" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="23" t="s">
+      <c r="C51" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="25"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="20"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
-      <c r="C52" s="19" t="s">
+      <c r="C52" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="23" t="s">
+      <c r="C53" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="25"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="20"/>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="18"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="18"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -1658,230 +1675,215 @@
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
+    <row r="58" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
+    <row r="59" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="10"/>
+      <c r="C59" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="7" t="s">
+    <row r="60" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="2"/>
+      <c r="C60" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="2"/>
+      <c r="C61" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
-      <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="10"/>
-      <c r="C61" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="2"/>
-      <c r="C62" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
-      <c r="C63" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="2"/>
-    </row>
-    <row r="64" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="2"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="2"/>
-    </row>
-    <row r="65" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="2"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="2"/>
-    </row>
-    <row r="66" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="2"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="2"/>
-    </row>
-    <row r="67" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="23"/>
+    </row>
+    <row r="66" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="10"/>
+      <c r="C66" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+    </row>
+    <row r="67" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="2"/>
-    </row>
-    <row r="68" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="2"/>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C68" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+    </row>
+    <row r="69" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C69" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="20"/>
+    </row>
+    <row r="70" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C70" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="20"/>
+    </row>
+    <row r="71" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D72" s="21"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-    </row>
-    <row r="73" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="10"/>
-      <c r="C73" s="19" t="s">
-        <v>102</v>
+      <c r="C71" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="20"/>
+    </row>
+    <row r="72" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="2"/>
+      <c r="C72" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="20"/>
+    </row>
+    <row r="73" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+      <c r="C73" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="D73" s="19"/>
       <c r="E73" s="19"/>
-      <c r="F73" s="19"/>
-    </row>
-    <row r="74" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="2"/>
-      <c r="C74" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="D74" s="27"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-    </row>
-    <row r="75" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="2"/>
-      <c r="C75" s="28"/>
-      <c r="D75" s="28"/>
-      <c r="E75" s="28"/>
-      <c r="F75" s="28"/>
-    </row>
-    <row r="76" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="2"/>
-      <c r="C76" s="16"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="18"/>
-    </row>
-    <row r="77" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="2"/>
-      <c r="C77" s="16"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="18"/>
-    </row>
-    <row r="78" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="2"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="18"/>
-    </row>
-    <row r="79" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="2"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="18"/>
-    </row>
-    <row r="80" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="2"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="18"/>
+      <c r="F73" s="20"/>
+    </row>
+    <row r="74" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+    </row>
+    <row r="75" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+    </row>
+    <row r="76" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+    </row>
+    <row r="77" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D77" s="16"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="26">
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="C76:F76"/>
     <mergeCell ref="C77:F77"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="C79:F79"/>
-    <mergeCell ref="C80:F80"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="C72:F72"/>
-    <mergeCell ref="C73:F73"/>
-    <mergeCell ref="C74:F74"/>
-    <mergeCell ref="C76:F76"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
     <mergeCell ref="H31:H32"/>
     <mergeCell ref="C51:F51"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C68:F68"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C54:F54"/>
-    <mergeCell ref="C55:F55"/>
+    <mergeCell ref="C59:F59"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C58:F58"/>
     <mergeCell ref="C61:F61"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C63:F63"/>
-    <mergeCell ref="C64:F64"/>
     <mergeCell ref="C65:F65"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C67:F67"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="C70:F70"/>
+    <mergeCell ref="C71:F71"/>
+    <mergeCell ref="C72:F72"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="C68:F68"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{58015AA5-94A6-4383-A3FD-6449A768BB7D}"/>
@@ -1903,5 +1905,6 @@
     <hyperlink ref="G42" r:id="rId17" location=":~:text=Dans%20l'univers%20SEO%2C%20schema,Google%20et%20Yahoo%20entre%20autres).&amp;text=Cette%20op%C3%A9ration%20a%20pour%20but,dans%20leur%20approche%20d'indexation." display="https://www.journaldunet.fr/web-tech/dictionnaire-du-webmastering/1203519-schema-org-definition/#:~:text=Dans%20l'univers%20SEO%2C%20schema,Google%20et%20Yahoo%20entre%20autres).&amp;text=Cette%20op%C3%A9ration%20a%20pour%20but,dans%20leur%20approche%20d'indexation." xr:uid="{52C84F2B-0474-430C-8117-A86EE01746F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>